<commit_message>
RdP et chatbot avril 2025
</commit_message>
<xml_diff>
--- a/Noyau RH FPE/7. DOCUMENTATION CHATBOT REBECCA/Chatbot Rebecca/Index_Newsletter.xlsx
+++ b/Noyau RH FPE/7. DOCUMENTATION CHATBOT REBECCA/Chatbot Rebecca/Index_Newsletter.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\balidfs1\onp\ONP\CISIRH\03-BARRI\REFERENTIELS\ASSISTANT VIRTUEL\4 - Communauté\5 - Portail BARRI [Doc Rebecca]\Documentation\Newsletter VF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\balidfs1\onp\ONP\CISIRH\03-BARRI\REFERENTIELS\ASSISTANT VIRTUEL\2. Communication\Portail BARRI [Doc Rebecca]\Documentation\Newsletter VF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02C674E-18CC-4048-8FB3-53E020835081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FC46B7-78AA-4CA7-9C8C-A87B86E36944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="18900" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INDEX!$B$2:$D$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INDEX!$B$2:$D$197</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="170">
   <si>
     <t>Plan de formation 1er semestre 2020</t>
   </si>
@@ -530,6 +530,24 @@
   </si>
   <si>
     <t>Migration de la communauté Osmose du chatbot Rebecca vers Resana</t>
+  </si>
+  <si>
+    <t>Mes réponses indemnitaires évoluent !</t>
+  </si>
+  <si>
+    <t>Mais où sont passées les 14 indemnités du Conseil d’État ?</t>
+  </si>
+  <si>
+    <t>Nouvelle version de la calculatrice des retenues à effectuer suite à un congé de maladie ordinaire à 90%</t>
+  </si>
+  <si>
+    <t>Congé de maladie ordinaire : le comptable n’attend plus de pièce justificative</t>
+  </si>
+  <si>
+    <t>L’enrichissement de la documentation PAY</t>
+  </si>
+  <si>
+    <t>L’ouverture de la communauté du chatbot Rebecca sur Resana, c’est fait !</t>
   </si>
 </sst>
 </file>
@@ -906,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D190"/>
+  <dimension ref="B1:D197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,7 +956,7 @@
     </row>
     <row r="3" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>81</v>
@@ -949,10 +967,10 @@
     </row>
     <row r="4" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D4" s="5">
         <v>2</v>
@@ -960,175 +978,175 @@
     </row>
     <row r="5" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D6" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7">
-        <v>45689</v>
+        <v>45748</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>81</v>
+        <v>167</v>
       </c>
       <c r="D7" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
-        <v>45689</v>
+        <v>45748</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D8" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
-        <v>45689</v>
+        <v>45748</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D9" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
+        <v>45717</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>45717</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
+        <v>45717</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>45717</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
         <v>45689</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D12" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D14" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>45627</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
-        <v>45627</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="D17" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D20" s="5">
         <v>3</v>
@@ -1136,109 +1154,109 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
-        <v>45597</v>
+        <v>45658</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D21" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
-        <v>45597</v>
+        <v>45658</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="D22" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D24" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D25" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D26" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="7">
-        <v>45566</v>
+        <v>45627</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D27" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D28" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D29" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D30" s="5">
         <v>3</v>
@@ -1246,252 +1264,252 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="7">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="D31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="7">
-        <v>45536</v>
+        <v>45597</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="D32" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D33" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D34" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D35" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="7">
-        <v>45474</v>
+        <v>45566</v>
       </c>
       <c r="C36" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
+        <v>45566</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
+        <v>45536</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D36" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="7">
-        <v>45474</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B38" s="7">
-        <v>45474</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="D38" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D39" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D40" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="7">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="D41" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="7">
-        <v>45444</v>
+        <v>45536</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D43" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D44" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D45" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="7">
-        <v>45413</v>
+        <v>45474</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D46" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="7">
-        <v>45413</v>
+        <v>45474</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D47" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="D48" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D49" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="7">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="D50" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="7">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D51" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="7">
-        <v>45383</v>
+        <v>45444</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D52" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="7">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
@@ -1499,32 +1517,32 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="7">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="D54" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="7">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D55" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="7">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D56" s="5">
         <v>3</v>
@@ -1532,7 +1550,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7">
-        <v>45292</v>
+        <v>45383</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>81</v>
@@ -1541,23 +1559,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="7">
-        <v>45292</v>
+        <v>45383</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D58" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="7">
-        <v>45292</v>
+        <v>45383</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D59" s="5">
         <v>2</v>
@@ -1565,98 +1583,98 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D60" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="D61" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="7">
-        <v>45261</v>
+        <v>45352</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="D62" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="7">
-        <v>45261</v>
+        <v>45352</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D63" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="D64" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D65" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="7">
-        <v>45231</v>
+        <v>45292</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>81</v>
+        <v>117</v>
       </c>
       <c r="D66" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="7">
-        <v>45231</v>
+        <v>45292</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="D67" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="7">
-        <v>45231</v>
+        <v>45292</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D68" s="5">
         <v>3</v>
@@ -1664,98 +1682,98 @@
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="7">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="D69" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="7">
-        <v>45200</v>
+        <v>45261</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="D70" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B71" s="7">
-        <v>45200</v>
+        <v>45261</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="D71" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="7">
-        <v>45200</v>
+        <v>45261</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D72" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D73" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D74" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D75" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="7">
-        <v>45170</v>
+        <v>45231</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="D76" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B77" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D77" s="5">
         <v>1</v>
@@ -1763,21 +1781,21 @@
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B78" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D78" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D79" s="5">
         <v>2</v>
@@ -1785,10 +1803,10 @@
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D80" s="5">
         <v>3</v>
@@ -1796,98 +1814,98 @@
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="7">
-        <v>45078</v>
+        <v>45200</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="D81" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="7">
-        <v>45078</v>
+        <v>45200</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D82" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B83" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D83" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B84" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D84" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B85" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D85" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B86" s="7">
-        <v>45047</v>
+        <v>45170</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="D86" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="7">
-        <v>45047</v>
+        <v>45170</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D87" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B88" s="7">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D88" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B89" s="7">
-        <v>45017</v>
+        <v>45078</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D89" s="5">
         <v>1</v>
@@ -1895,32 +1913,32 @@
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="7">
-        <v>45017</v>
+        <v>45078</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D90" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B91" s="7">
-        <v>45017</v>
+        <v>45078</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D91" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B92" s="7">
-        <v>45017</v>
+        <v>45078</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D92" s="5">
         <v>3</v>
@@ -1928,43 +1946,43 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B93" s="7">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D93" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B94" s="7">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D94" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B95" s="7">
-        <v>44986</v>
+        <v>45047</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D95" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D96" s="5">
         <v>1</v>
@@ -1972,21 +1990,21 @@
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D97" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D98" s="5">
         <v>2</v>
@@ -1994,32 +2012,32 @@
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="7">
-        <v>44958</v>
+        <v>45017</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D99" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="7">
-        <v>44958</v>
+        <v>45017</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="D100" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="7">
-        <v>44958</v>
+        <v>45017</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D101" s="5">
         <v>3</v>
@@ -2027,21 +2045,21 @@
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="7">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D102" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="7">
-        <v>44927</v>
+        <v>44986</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="D103" s="5">
         <v>1</v>
@@ -2049,21 +2067,21 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="7">
-        <v>44927</v>
+        <v>44986</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D104" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="7">
-        <v>44927</v>
+        <v>44986</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D105" s="5">
         <v>2</v>
@@ -2071,362 +2089,362 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D106" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B107" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D107" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B108" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D108" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B109" s="7">
-        <v>44866</v>
+        <v>44958</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D109" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>73</v>
+        <v>38</v>
       </c>
       <c r="D110" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D111" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B112" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D112" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B113" s="7">
-        <v>44835</v>
+        <v>44927</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="D113" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="7">
-        <v>44835</v>
+        <v>44927</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="D114" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="7">
-        <v>44835</v>
+        <v>44927</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D115" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D116" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D117" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="7">
+        <v>44866</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D118" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="7">
+        <v>44866</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D119" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="7">
         <v>44835</v>
       </c>
-      <c r="C118" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D118" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="7">
-        <v>44743</v>
-      </c>
-      <c r="C119" s="4" t="s">
+      <c r="C120" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D119" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B120" s="7">
-        <v>44743</v>
-      </c>
-      <c r="C120" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="D120" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B121" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D121" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B122" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D122" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D123" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" s="7">
-        <v>44682</v>
+        <v>44835</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="D124" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" s="7">
-        <v>44682</v>
+        <v>44835</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D125" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="D126" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B127" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D127" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D128" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="7">
-        <v>44621</v>
+        <v>44743</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="D129" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B130" s="7">
-        <v>44621</v>
+        <v>44743</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D130" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D131" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B132" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D132" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B133" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D133" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B134" s="7">
-        <v>44593</v>
+        <v>44682</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D134" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B135" s="7">
-        <v>44593</v>
+        <v>44682</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D135" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B136" s="7">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D136" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B137" s="7">
-        <v>44531</v>
+        <v>44621</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D137" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B138" s="7">
-        <v>44531</v>
+        <v>44621</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D138" s="5">
         <v>2</v>
@@ -2434,153 +2452,153 @@
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B139" s="7">
-        <v>44531</v>
+        <v>44621</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D139" s="9">
-        <v>5</v>
+        <v>56</v>
+      </c>
+      <c r="D139" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B140" s="7">
-        <v>44531</v>
+        <v>44621</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D140" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="141" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D140" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B141" s="7">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D141" s="9" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="D141" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B142" s="7">
-        <v>44470</v>
+        <v>44593</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D142" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B143" s="7">
-        <v>44470</v>
+        <v>44593</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D143" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B144" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D144" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D145" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="7">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D146" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D146" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B147" s="7">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D147" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D147" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B148" s="7">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D148" s="5">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="7">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D149" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" s="7">
-        <v>44317</v>
+        <v>44470</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D150" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" s="7">
-        <v>44317</v>
+        <v>44470</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D151" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" s="7">
-        <v>44317</v>
+        <v>44470</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D152" s="5">
         <v>3</v>
@@ -2588,208 +2606,208 @@
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B153" s="7">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D153" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B154" s="7">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D154" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B155" s="7">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D155" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B156" s="7">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D156" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B157" s="7">
-        <v>44228</v>
+        <v>44317</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D157" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B158" s="7">
-        <v>44166</v>
+        <v>44317</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D158" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B159" s="7">
-        <v>44166</v>
+        <v>44317</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D159" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B160" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D160" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D161" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B162" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D162" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" s="7">
-        <v>44105</v>
+        <v>44228</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D163" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" s="7">
-        <v>44105</v>
+        <v>44228</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D164" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D165" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D166" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" s="7">
-        <v>44075</v>
+        <v>44166</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D167" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B168" s="7">
-        <v>44075</v>
+        <v>44166</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D168" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" s="7">
-        <v>44075</v>
+        <v>44166</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D169" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B170" s="7">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D170" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="7">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D171" s="5">
         <v>1</v>
@@ -2797,29 +2815,29 @@
     </row>
     <row r="172" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B172" s="7">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D172" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B173" s="7">
-        <v>44013</v>
+        <v>44105</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D173" s="8" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="D173" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="174" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B174" s="7">
-        <v>43983</v>
+        <v>44075</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>12</v>
@@ -2830,10 +2848,10 @@
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="7">
-        <v>43983</v>
+        <v>44075</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D175" s="5">
         <v>1</v>
@@ -2841,10 +2859,10 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B176" s="7">
-        <v>43983</v>
+        <v>44075</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D176" s="5">
         <v>2</v>
@@ -2852,10 +2870,10 @@
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B177" s="7">
-        <v>43983</v>
+        <v>44075</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D177" s="5">
         <v>3</v>
@@ -2863,7 +2881,7 @@
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B178" s="7">
-        <v>43952</v>
+        <v>44013</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>12</v>
@@ -2874,43 +2892,43 @@
     </row>
     <row r="179" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B179" s="7">
-        <v>43952</v>
+        <v>44013</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D179" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B180" s="7">
-        <v>43952</v>
+        <v>44013</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D180" s="5">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="D180" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B181" s="7">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D181" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" s="7">
-        <v>43891</v>
+        <v>43983</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D182" s="5">
         <v>1</v>
@@ -2918,94 +2936,171 @@
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B183" s="7">
-        <v>43891</v>
+        <v>43983</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D183" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B184" s="7">
-        <v>43891</v>
+        <v>43983</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D184" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B185" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D185" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D186" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" s="7">
-        <v>43862</v>
+        <v>43952</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D187" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" s="7">
-        <v>43862</v>
+        <v>43952</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D188" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B189" s="7">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D189" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="7">
+        <v>43891</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D190" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="7">
+        <v>43891</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D191" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="7">
+        <v>43891</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D192" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="7">
+        <v>43891</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="7">
         <v>43862</v>
       </c>
-      <c r="C190" s="4" t="s">
+      <c r="C194" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D194" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D195" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D196" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C197" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D190" s="5">
+      <c r="D197" s="5">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D190" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B2:D197" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MAJ chatbot Rebecca février 2026
</commit_message>
<xml_diff>
--- a/Noyau RH FPE/7. DOCUMENTATION CHATBOT REBECCA/Chatbot Rebecca/Index_Newsletter.xlsx
+++ b/Noyau RH FPE/7. DOCUMENTATION CHATBOT REBECCA/Chatbot Rebecca/Index_Newsletter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\03-BARRI\REFERENTIELS\ASSISTANT VIRTUEL\2 - Communication\Portail BARRI [Doc Rebecca]\Documentation\Newsletter VF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7B8B5F-D049-47A4-B806-781740B7DD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C45F3B-3E17-4AF6-BEC4-F2276E68364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INDEX!$B$2:$D$236</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">INDEX!$B$2:$D$240</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="206">
   <si>
     <t>Plan de formation 1er semestre 2020</t>
   </si>
@@ -647,6 +647,18 @@
   </si>
   <si>
     <t>Retour en images sur ma participation au salon des applications RH</t>
+  </si>
+  <si>
+    <t>Consultez mes principales notifications en un seul clic !</t>
+  </si>
+  <si>
+    <t>Nouvelle présentation des indemnités déclinées</t>
+  </si>
+  <si>
+    <t>Du plus pour les gestionnaires du ministère de la transition écologique !</t>
+  </si>
+  <si>
+    <t>Mes réponses s’enrichissent pour faciliter votre saisie dans le SIRH</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D236"/>
+  <dimension ref="B1:D240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,10 +1088,10 @@
     </row>
     <row r="3" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="7">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>202</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -1087,10 +1099,10 @@
     </row>
     <row r="4" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D4" s="5">
         <v>2</v>
@@ -1098,10 +1110,10 @@
     </row>
     <row r="5" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D5" s="5">
         <v>3</v>
@@ -1109,10 +1121,10 @@
     </row>
     <row r="6" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="7">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D6" s="5">
         <v>4</v>
@@ -1123,76 +1135,76 @@
         <v>46023</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>200</v>
+        <v>81</v>
       </c>
       <c r="D7" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7">
         <v>46023</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" s="13">
-        <v>5</v>
+      <c r="C8" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>95</v>
+        <v>198</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="7">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7">
-        <v>45992</v>
+        <v>46023</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="D11" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7">
-        <v>45992</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D12" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>46023</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="7">
         <v>45992</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>195</v>
+        <v>95</v>
       </c>
       <c r="D13" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1200,54 +1212,54 @@
         <v>45992</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D14" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="7">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="7">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B18" s="7">
-        <v>45962</v>
+        <v>45992</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1255,18 +1267,18 @@
         <v>45962</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>191</v>
+        <v>95</v>
       </c>
       <c r="D19" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="7">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>81</v>
+        <v>188</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -1274,21 +1286,21 @@
     </row>
     <row r="21" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="7">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D21" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="7">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D22" s="5">
         <v>3</v>
@@ -1296,76 +1308,76 @@
     </row>
     <row r="23" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="7">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D23" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="7">
         <v>45931</v>
       </c>
-      <c r="C24" t="s">
-        <v>187</v>
+      <c r="C24" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="D24" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="7">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D25" s="11">
-        <v>1</v>
+        <v>184</v>
+      </c>
+      <c r="D25" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="7">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="11">
-        <v>2</v>
+        <v>185</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="7">
-        <v>45901</v>
+        <v>45931</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D27" s="11">
-        <v>2</v>
+        <v>186</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="7">
-        <v>45901</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" s="11">
-        <v>3</v>
+        <v>45931</v>
+      </c>
+      <c r="C28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D28" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7">
-        <v>45839</v>
+        <v>45901</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>180</v>
       </c>
       <c r="D29" s="11">
         <v>1</v>
@@ -1373,21 +1385,21 @@
     </row>
     <row r="30" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B30" s="7">
-        <v>45839</v>
+        <v>45901</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D30" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B31" s="7">
-        <v>45839</v>
+        <v>45901</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D31" s="11">
         <v>2</v>
@@ -1395,10 +1407,10 @@
     </row>
     <row r="32" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="7">
-        <v>45839</v>
+        <v>45901</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D32" s="11">
         <v>3</v>
@@ -1409,18 +1421,18 @@
         <v>45839</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>179</v>
+        <v>86</v>
       </c>
       <c r="D33" s="11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>81</v>
+        <v>176</v>
       </c>
       <c r="D34" s="11">
         <v>1</v>
@@ -1428,10 +1440,10 @@
     </row>
     <row r="35" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B35" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D35" s="11">
         <v>2</v>
@@ -1439,10 +1451,10 @@
     </row>
     <row r="36" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B36" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D36" s="11">
         <v>3</v>
@@ -1450,43 +1462,43 @@
     </row>
     <row r="37" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B37" s="7">
-        <v>45778</v>
+        <v>45839</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="D37" s="11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B38" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>170</v>
+        <v>81</v>
       </c>
       <c r="D38" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B39" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D39" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B40" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D40" s="11">
         <v>3</v>
@@ -1497,53 +1509,53 @@
         <v>45778</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>173</v>
+        <v>95</v>
       </c>
       <c r="D41" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B42" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="5">
-        <v>1</v>
+        <v>170</v>
+      </c>
+      <c r="D42" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B43" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D43" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+      <c r="D43" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D44" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+      <c r="D44" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B45" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D45" s="5">
+        <v>173</v>
+      </c>
+      <c r="D45" s="11">
         <v>3</v>
       </c>
     </row>
@@ -1552,10 +1564,10 @@
         <v>45748</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="D46" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1563,10 +1575,10 @@
         <v>45748</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D47" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1574,51 +1586,51 @@
         <v>45748</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D48" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="D49" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D50" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B51" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D51" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B52" s="7">
-        <v>45717</v>
+        <v>45748</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D52" s="5">
         <v>4</v>
@@ -1626,7 +1638,7 @@
     </row>
     <row r="53" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B53" s="7">
-        <v>45689</v>
+        <v>45717</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>81</v>
@@ -1637,10 +1649,10 @@
     </row>
     <row r="54" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B54" s="7">
-        <v>45689</v>
+        <v>45717</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D54" s="5">
         <v>2</v>
@@ -1648,10 +1660,10 @@
     </row>
     <row r="55" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B55" s="7">
-        <v>45689</v>
+        <v>45717</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D55" s="5">
         <v>3</v>
@@ -1659,57 +1671,57 @@
     </row>
     <row r="56" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="7">
+        <v>45717</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="7">
         <v>45689</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C57" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="7">
+        <v>45689</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D56" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D58" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B59" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D59" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B60" s="7">
-        <v>45658</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="D60" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.35">
@@ -1717,106 +1729,106 @@
         <v>45658</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D61" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="D62" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="D63" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="D64" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B65" s="7">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D65" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="7">
         <v>45627</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="D66" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B67" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D67" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D68" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D69" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B70" s="7">
-        <v>45597</v>
+        <v>45627</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D70" s="5">
         <v>3</v>
@@ -1827,84 +1839,84 @@
         <v>45597</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D71" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D72" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D73" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D74" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B75" s="7">
-        <v>45566</v>
+        <v>45597</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D75" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="7">
         <v>45566</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D76" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="D77" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D78" s="5">
         <v>2</v>
@@ -1912,24 +1924,24 @@
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B79" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="D79" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B80" s="7">
-        <v>45536</v>
+        <v>45566</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D80" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.35">
@@ -1937,54 +1949,54 @@
         <v>45536</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="D81" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B82" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="D82" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D83" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D84" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="7">
-        <v>45474</v>
+        <v>45536</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D85" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.35">
@@ -1992,18 +2004,18 @@
         <v>45474</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="D86" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D87" s="5">
         <v>1</v>
@@ -2011,35 +2023,35 @@
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D88" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D89" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" s="7">
-        <v>45444</v>
+        <v>45474</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D90" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.35">
@@ -2047,18 +2059,18 @@
         <v>45444</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="D91" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="D92" s="5">
         <v>1</v>
@@ -2066,10 +2078,10 @@
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D93" s="5">
         <v>2</v>
@@ -2077,10 +2089,10 @@
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D94" s="5">
         <v>3</v>
@@ -2088,10 +2100,10 @@
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B95" s="7">
-        <v>45413</v>
+        <v>45444</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D95" s="5">
         <v>3</v>
@@ -2099,7 +2111,7 @@
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B96" s="7">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>81</v>
@@ -2108,78 +2120,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B97" s="7">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D97" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B98" s="7">
-        <v>45383</v>
+        <v>45413</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D98" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B99" s="7">
-        <v>45352</v>
+        <v>45413</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D99" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B100" s="7">
-        <v>45352</v>
+        <v>45383</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D100" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B101" s="7">
-        <v>45352</v>
+        <v>45383</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D101" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B102" s="7">
-        <v>45352</v>
+        <v>45383</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D102" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="D103" s="5">
         <v>1</v>
@@ -2187,21 +2199,21 @@
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="D104" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B105" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D105" s="5">
         <v>2</v>
@@ -2209,10 +2221,10 @@
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106" s="7">
-        <v>45292</v>
+        <v>45352</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D106" s="5">
         <v>3</v>
@@ -2223,29 +2235,29 @@
         <v>45292</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="D107" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
       <c r="D108" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D109" s="5">
         <v>2</v>
@@ -2253,21 +2265,21 @@
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D110" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B111" s="7">
-        <v>45261</v>
+        <v>45292</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D111" s="5">
         <v>3</v>
@@ -2275,7 +2287,7 @@
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B112" s="7">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>81</v>
@@ -2284,12 +2296,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113" s="7">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D113" s="5">
         <v>2</v>
@@ -2297,21 +2309,21 @@
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="7">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D114" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B115" s="7">
-        <v>45231</v>
+        <v>45261</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D115" s="5">
         <v>3</v>
@@ -2319,43 +2331,43 @@
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B116" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D116" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B117" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D117" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B118" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D118" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B119" s="7">
-        <v>45200</v>
+        <v>45231</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D119" s="5">
         <v>3</v>
@@ -2366,10 +2378,10 @@
         <v>45200</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D120" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.35">
@@ -2377,54 +2389,54 @@
         <v>45200</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D121" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B122" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D122" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B123" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D123" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B124" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D124" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B125" s="7">
-        <v>45170</v>
+        <v>45200</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D125" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.35">
@@ -2432,18 +2444,18 @@
         <v>45170</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D126" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B127" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D127" s="5">
         <v>1</v>
@@ -2451,21 +2463,21 @@
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B128" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D128" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B129" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D129" s="5">
         <v>2</v>
@@ -2473,10 +2485,10 @@
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B130" s="7">
-        <v>45078</v>
+        <v>45170</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D130" s="5">
         <v>3</v>
@@ -2487,18 +2499,18 @@
         <v>45078</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D131" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B132" s="7">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="D132" s="5">
         <v>1</v>
@@ -2506,10 +2518,10 @@
     </row>
     <row r="133" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B133" s="7">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D133" s="5">
         <v>2</v>
@@ -2517,10 +2529,10 @@
     </row>
     <row r="134" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B134" s="7">
-        <v>45047</v>
+        <v>45078</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D134" s="5">
         <v>3</v>
@@ -2528,21 +2540,21 @@
     </row>
     <row r="135" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B135" s="7">
-        <v>45017</v>
+        <v>45078</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="D135" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B136" s="7">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D136" s="5">
         <v>1</v>
@@ -2550,10 +2562,10 @@
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B137" s="7">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D137" s="5">
         <v>2</v>
@@ -2561,10 +2573,10 @@
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B138" s="7">
-        <v>45017</v>
+        <v>45047</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D138" s="5">
         <v>3</v>
@@ -2575,10 +2587,10 @@
         <v>45017</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D139" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.35">
@@ -2586,62 +2598,62 @@
         <v>45017</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D140" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B141" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D141" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B142" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D142" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B143" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D143" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B144" s="7">
-        <v>44986</v>
+        <v>45017</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D144" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B145" s="7">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D145" s="5">
         <v>1</v>
@@ -2649,43 +2661,43 @@
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B146" s="7">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D146" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B147" s="7">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D147" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B148" s="7">
-        <v>44958</v>
+        <v>44986</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D148" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B149" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="D149" s="5">
         <v>1</v>
@@ -2693,35 +2705,35 @@
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B150" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D150" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B151" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D151" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B152" s="7">
-        <v>44927</v>
+        <v>44958</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D152" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="2:4" x14ac:dyDescent="0.35">
@@ -2729,10 +2741,10 @@
         <v>44927</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>79</v>
+        <v>38</v>
       </c>
       <c r="D153" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.35">
@@ -2740,73 +2752,73 @@
         <v>44927</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D154" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B155" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D155" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B156" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D156" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B157" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D157" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B158" s="7">
-        <v>44866</v>
+        <v>44927</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D158" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B159" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="D159" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B160" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D160" s="5">
         <v>2</v>
@@ -2814,21 +2826,21 @@
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D161" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="7">
-        <v>44835</v>
+        <v>44866</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D162" s="5">
         <v>3</v>
@@ -2839,139 +2851,139 @@
         <v>44835</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="D163" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B164" s="7">
         <v>44835</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D164" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D165" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D166" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D167" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="7">
-        <v>44743</v>
+        <v>44835</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D168" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B169" s="7">
         <v>44743</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D169" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D170" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D171" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B172" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D172" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="7">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D173" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B174" s="7">
         <v>44682</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D174" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D175" s="5">
         <v>1</v>
@@ -2979,10 +2991,10 @@
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D176" s="5">
         <v>2</v>
@@ -2990,21 +3002,21 @@
     </row>
     <row r="177" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B177" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D177" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B178" s="7">
-        <v>44621</v>
+        <v>44682</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D178" s="5">
         <v>3</v>
@@ -3015,29 +3027,29 @@
         <v>44621</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D179" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B180" s="7">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D180" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B181" s="7">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D181" s="5">
         <v>2</v>
@@ -3045,10 +3057,10 @@
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B182" s="7">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D182" s="5">
         <v>3</v>
@@ -3056,106 +3068,106 @@
     </row>
     <row r="183" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B183" s="7">
-        <v>44531</v>
+        <v>44621</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="D183" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B184" s="7">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D184" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B185" s="7">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D185" s="9">
-        <v>5</v>
+        <v>52</v>
+      </c>
+      <c r="D185" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B186" s="7">
-        <v>44531</v>
+        <v>44593</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D186" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="D186" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B187" s="7">
         <v>44531</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D187" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="D187" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B188" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D188" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B189" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D189" s="5">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="D189" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B190" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D190" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="D190" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B191" s="7">
-        <v>44470</v>
+        <v>44531</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D191" s="5">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="D191" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B192" s="7">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>38</v>
@@ -3164,12 +3176,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="7">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D193" s="5">
         <v>2</v>
@@ -3177,10 +3189,10 @@
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="7">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D194" s="5">
         <v>3</v>
@@ -3188,10 +3200,10 @@
     </row>
     <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="7">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D195" s="5">
         <v>3</v>
@@ -3199,7 +3211,7 @@
     </row>
     <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="7">
-        <v>44317</v>
+        <v>44378</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>38</v>
@@ -3208,12 +3220,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B197" s="7">
-        <v>44317</v>
+        <v>44378</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D197" s="5">
         <v>2</v>
@@ -3221,10 +3233,10 @@
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="7">
-        <v>44317</v>
+        <v>44378</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D198" s="5">
         <v>3</v>
@@ -3232,32 +3244,32 @@
     </row>
     <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="7">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D199" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="7">
-        <v>44228</v>
+        <v>44317</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D200" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="7">
-        <v>44228</v>
+        <v>44317</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D201" s="5">
         <v>2</v>
@@ -3265,13 +3277,13 @@
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="7">
-        <v>44228</v>
+        <v>44317</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D202" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.35">
@@ -3279,40 +3291,40 @@
         <v>44228</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D203" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D204" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B205" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D205" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D206" s="5">
         <v>2</v>
@@ -3320,10 +3332,10 @@
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="7">
-        <v>44166</v>
+        <v>44228</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D207" s="5">
         <v>3</v>
@@ -3334,18 +3346,18 @@
         <v>44166</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D208" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B209" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D209" s="5">
         <v>1</v>
@@ -3353,32 +3365,32 @@
     </row>
     <row r="210" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B210" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D210" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B211" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D211" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="212" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B212" s="7">
-        <v>44105</v>
+        <v>44166</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D212" s="5">
         <v>3</v>
@@ -3386,7 +3398,7 @@
     </row>
     <row r="213" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B213" s="7">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>12</v>
@@ -3397,10 +3409,10 @@
     </row>
     <row r="214" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B214" s="7">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D214" s="5">
         <v>1</v>
@@ -3408,21 +3420,21 @@
     </row>
     <row r="215" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B215" s="7">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D215" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="216" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B216" s="7">
-        <v>44075</v>
+        <v>44105</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D216" s="5">
         <v>3</v>
@@ -3430,7 +3442,7 @@
     </row>
     <row r="217" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B217" s="7">
-        <v>44013</v>
+        <v>44075</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>12</v>
@@ -3441,43 +3453,43 @@
     </row>
     <row r="218" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B218" s="7">
-        <v>44013</v>
+        <v>44075</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D218" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="219" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B219" s="7">
-        <v>44013</v>
+        <v>44075</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D219" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="D219" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B220" s="7">
-        <v>43983</v>
+        <v>44075</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D220" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B221" s="7">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D221" s="5">
         <v>1</v>
@@ -3485,29 +3497,29 @@
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B222" s="7">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="C222" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D222" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B223" s="7">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D223" s="5">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="D223" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="224" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B224" s="7">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>12</v>
@@ -3518,10 +3530,10 @@
     </row>
     <row r="225" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B225" s="7">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D225" s="5">
         <v>1</v>
@@ -3529,10 +3541,10 @@
     </row>
     <row r="226" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B226" s="7">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D226" s="5">
         <v>2</v>
@@ -3540,10 +3552,10 @@
     </row>
     <row r="227" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B227" s="7">
-        <v>43952</v>
+        <v>43983</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D227" s="5">
         <v>3</v>
@@ -3551,10 +3563,10 @@
     </row>
     <row r="228" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B228" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D228" s="5">
         <v>1</v>
@@ -3562,10 +3574,10 @@
     </row>
     <row r="229" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B229" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D229" s="5">
         <v>1</v>
@@ -3573,10 +3585,10 @@
     </row>
     <row r="230" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B230" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D230" s="5">
         <v>2</v>
@@ -3584,10 +3596,10 @@
     </row>
     <row r="231" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B231" s="7">
-        <v>43891</v>
+        <v>43952</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D231" s="5">
         <v>3</v>
@@ -3598,18 +3610,18 @@
         <v>43891</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D232" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B233" s="7">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D233" s="5">
         <v>1</v>
@@ -3617,10 +3629,10 @@
     </row>
     <row r="234" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B234" s="7">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D234" s="5">
         <v>2</v>
@@ -3628,28 +3640,72 @@
     </row>
     <row r="235" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B235" s="7">
-        <v>43862</v>
+        <v>43891</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D235" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="236" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B236" s="7">
+        <v>43891</v>
+      </c>
+      <c r="C236" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D236" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B237" s="7">
         <v>43862</v>
       </c>
-      <c r="C236" s="4" t="s">
+      <c r="C237" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D237" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B238" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C238" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D238" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B239" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C239" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D239" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B240" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C240" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D236" s="5">
+      <c r="D240" s="5">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:D236" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="B2:D240" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>